<commit_message>
Extending the doughnut chart
</commit_message>
<xml_diff>
--- a/Hugo/sites/M365Blog/content/posts/images/doughnut-chart/Doughnut-Chart_v1.xlsx
+++ b/Hugo/sites/M365Blog/content/posts/images/doughnut-chart/Doughnut-Chart_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\auckloor\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reshm\source\repos\blogs\Hugo\sites\M365Blog\content\posts\images\doughnut-chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC143B74-11F1-4DCF-980F-73B2D06BDFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38079F25-8392-4ACA-8681-7CC6E3ECE222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="query (3)" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Title</t>
   </si>
@@ -136,36 +136,12 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Days to Take</t>
-  </si>
-  <si>
     <t>#1b429a</t>
   </si>
   <si>
-    <t>Volunteering days by Directorates for 2023-2024</t>
-  </si>
-  <si>
-    <t>Business Support</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HROD </t>
-  </si>
-  <si>
     <t>Investment</t>
   </si>
   <si>
-    <t>Risk and Compliance</t>
-  </si>
-  <si>
-    <t>Scheme &amp; Member Services</t>
-  </si>
-  <si>
-    <t>Strategy and Legal Affairs</t>
-  </si>
-  <si>
-    <t>Technology and Change Services</t>
-  </si>
-  <si>
     <t>LABEL8</t>
   </si>
   <si>
@@ -185,6 +161,33 @@
   </si>
   <si>
     <t>VALUE9</t>
+  </si>
+  <si>
+    <t>Volunteering days by departments for 2023-2024</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Customer Service</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>Sustainability</t>
+  </si>
+  <si>
+    <t>Diversity &amp; Inclusion</t>
   </si>
 </sst>
 </file>
@@ -674,10 +677,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -725,27 +727,9 @@
   </cellStyles>
   <dxfs count="26">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -765,6 +749,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -786,6 +779,15 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -882,28 +884,28 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="LABEL4" name="LABEL4" queryTableFieldId="8" dataDxfId="21"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="LABEL5" name="LABEL5" queryTableFieldId="9" dataDxfId="20"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="LABEL6" name="LABEL6" queryTableFieldId="10" dataDxfId="19"/>
-    <tableColumn id="26" xr3:uid="{BAC5AAA6-B50A-4DDC-BDB7-D60705029923}" uniqueName="26" name="LABEL7" queryTableFieldId="28" dataDxfId="2"/>
-    <tableColumn id="25" xr3:uid="{84E40EE8-2471-4699-AC8F-62D87FA35D92}" uniqueName="25" name="LABEL8" queryTableFieldId="27" dataDxfId="3"/>
-    <tableColumn id="21" xr3:uid="{A140B053-D5B5-43F4-A5EA-A6D25A5D65FE}" uniqueName="21" name="LABEL9" queryTableFieldId="23" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="COLOR1" name="COLOR1" queryTableFieldId="17" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="COLOR2" name="COLOR2" queryTableFieldId="18" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" uniqueName="COLOR3" name="COLOR3" queryTableFieldId="19" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" uniqueName="COLOR4" name="COLOR4" queryTableFieldId="20" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" uniqueName="COLOR5" name="COLOR5" queryTableFieldId="21" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" uniqueName="COLOR6" name="COLOR6" queryTableFieldId="22" dataDxfId="13"/>
-    <tableColumn id="28" xr3:uid="{C4E7D29F-82BA-4EB5-8385-F36E6116B4B4}" uniqueName="28" name="COLOR7" queryTableFieldId="30" dataDxfId="0"/>
-    <tableColumn id="27" xr3:uid="{F11AAED7-EF3F-44AE-9CB2-C934F88544A5}" uniqueName="27" name="COLOR8" queryTableFieldId="29" dataDxfId="1"/>
-    <tableColumn id="22" xr3:uid="{8B77C3BC-6913-4D17-B196-7F4A6AC76D46}" uniqueName="22" name="COLOR9" queryTableFieldId="24" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" uniqueName="VALUE1" name="VALUE1" queryTableFieldId="11" dataDxfId="12"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" uniqueName="VALUE2" name="VALUE2" queryTableFieldId="12" dataDxfId="11"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" uniqueName="VALUE3" name="VALUE3" queryTableFieldId="13" dataDxfId="10"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="VALUE4" name="VALUE4" queryTableFieldId="14" dataDxfId="9"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" uniqueName="VALUE5" name="VALUE5" queryTableFieldId="15" dataDxfId="8"/>
+    <tableColumn id="26" xr3:uid="{BAC5AAA6-B50A-4DDC-BDB7-D60705029923}" uniqueName="26" name="LABEL7" queryTableFieldId="28" dataDxfId="18"/>
+    <tableColumn id="25" xr3:uid="{84E40EE8-2471-4699-AC8F-62D87FA35D92}" uniqueName="25" name="LABEL8" queryTableFieldId="27" dataDxfId="17"/>
+    <tableColumn id="21" xr3:uid="{A140B053-D5B5-43F4-A5EA-A6D25A5D65FE}" uniqueName="21" name="LABEL9" queryTableFieldId="23" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="COLOR1" name="COLOR1" queryTableFieldId="17" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="COLOR2" name="COLOR2" queryTableFieldId="18" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" uniqueName="COLOR3" name="COLOR3" queryTableFieldId="19" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" uniqueName="COLOR4" name="COLOR4" queryTableFieldId="20" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" uniqueName="COLOR5" name="COLOR5" queryTableFieldId="21" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" uniqueName="COLOR6" name="COLOR6" queryTableFieldId="22" dataDxfId="10"/>
+    <tableColumn id="28" xr3:uid="{C4E7D29F-82BA-4EB5-8385-F36E6116B4B4}" uniqueName="28" name="COLOR7" queryTableFieldId="30" dataDxfId="9"/>
+    <tableColumn id="27" xr3:uid="{F11AAED7-EF3F-44AE-9CB2-C934F88544A5}" uniqueName="27" name="COLOR8" queryTableFieldId="29" dataDxfId="8"/>
+    <tableColumn id="22" xr3:uid="{8B77C3BC-6913-4D17-B196-7F4A6AC76D46}" uniqueName="22" name="COLOR9" queryTableFieldId="24" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" uniqueName="VALUE1" name="VALUE1" queryTableFieldId="11" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" uniqueName="VALUE2" name="VALUE2" queryTableFieldId="12" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" uniqueName="VALUE3" name="VALUE3" queryTableFieldId="13" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="VALUE4" name="VALUE4" queryTableFieldId="14" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" uniqueName="VALUE5" name="VALUE5" queryTableFieldId="15" dataDxfId="2"/>
     <tableColumn id="30" xr3:uid="{56082882-F44D-43A1-88E4-AA5816C4FF78}" uniqueName="30" name="VALUE6" queryTableFieldId="32"/>
     <tableColumn id="29" xr3:uid="{D0E09413-F6C5-4C8E-8265-0517DCBCFD30}" uniqueName="29" name="VALUE7" queryTableFieldId="31"/>
     <tableColumn id="23" xr3:uid="{D538C46C-E609-4F42-8EC3-00316AC2E0E5}" uniqueName="23" name="VALUE8" queryTableFieldId="25"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" uniqueName="VALUE6" name="VALUE9" queryTableFieldId="16" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{5B39D5C0-5F1E-477F-8C84-0AC1E04AEB84}" uniqueName="24" name="TOTAL" queryTableFieldId="26" dataDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" uniqueName="VALUE6" name="VALUE9" queryTableFieldId="16" dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{5B39D5C0-5F1E-477F-8C84-0AC1E04AEB84}" uniqueName="24" name="TOTAL" queryTableFieldId="26" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1208,31 +1210,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7265625" customWidth="1"/>
+    <col min="9" max="9" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="11" max="16" width="10" bestFit="1" customWidth="1"/>
     <col min="17" max="19" width="10" customWidth="1"/>
-    <col min="20" max="24" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="9.85546875" customWidth="1"/>
-    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="9.85546875" customWidth="1"/>
+    <col min="20" max="24" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="9.81640625" customWidth="1"/>
+    <col min="28" max="28" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1258,10 +1260,10 @@
         <v>25</v>
       </c>
       <c r="I1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K1" t="s">
         <v>13</v>
@@ -1285,10 +1287,10 @@
         <v>26</v>
       </c>
       <c r="R1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="S1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="T1" t="s">
         <v>7</v>
@@ -1315,42 +1317,42 @@
         <v>28</v>
       </c>
       <c r="AB1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="AC1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>19</v>
@@ -1371,13 +1373,13 @@
         <v>24</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T2">
         <v>10</v>
@@ -1407,7 +1409,7 @@
         <f>500-Tabella_query__3[[#This Row],[VALUE1]]-Tabella_query__3[[#This Row],[VALUE2]]-Tabella_query__3[[#This Row],[VALUE3]]-Tabella_query__3[[#This Row],[VALUE4]]-Tabella_query__3[[#This Row],[VALUE5]]-Tabella_query__3[[#This Row],[VALUE6]]-Tabella_query__3[[#This Row],[VALUE7]]-Tabella_query__3[[#This Row],[VALUE8]]</f>
         <v>373</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AC2">
         <v>500</v>
       </c>
     </row>

</xml_diff>